<commit_message>
Added items to the sprint1 backlog
</commit_message>
<xml_diff>
--- a/assignment8/src/Backlog/Sprint 1 Backlog.xlsx
+++ b/assignment8/src/Backlog/Sprint 1 Backlog.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10425" windowHeight="2880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Very High</t>
   </si>
@@ -68,6 +69,30 @@
   </si>
   <si>
     <t>Do part 1 of assignment-8</t>
+  </si>
+  <si>
+    <t>Create testcase for Calculation to compute Time</t>
+  </si>
+  <si>
+    <t>Create testcase for Calculation to compute distance</t>
+  </si>
+  <si>
+    <t>Create testcase for Calculation to compute pace</t>
+  </si>
+  <si>
+    <t>Build user interface-window.java (Windows Builder)</t>
+  </si>
+  <si>
+    <t>build Class Distance.java</t>
+  </si>
+  <si>
+    <t>build Class Pace.java</t>
+  </si>
+  <si>
+    <t>build Class Time.java</t>
+  </si>
+  <si>
+    <t>build class PaceCalculator.java</t>
   </si>
 </sst>
 </file>
@@ -527,16 +552,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="44" style="13" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="13" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
   </cols>
@@ -677,24 +702,103 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="B11" s="9">
+        <v>8</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1</v>
+      </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+      <c r="B12" s="9">
+        <v>9</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
       <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="B13" s="9">
+        <v>10</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
       <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="13">
+        <v>11</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="13">
+        <v>12</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="13">
+        <v>13</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="13">
+        <v>14</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="13">
+        <v>15</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated assigned column for test cases. Added day 2 status
</commit_message>
<xml_diff>
--- a/assignment8/src/Backlog/Sprint 1 Backlog.xlsx
+++ b/assignment8/src/Backlog/Sprint 1 Backlog.xlsx
@@ -10,12 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Very High</t>
   </si>
@@ -554,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,7 +710,9 @@
       <c r="D11" s="9">
         <v>1</v>
       </c>
-      <c r="E11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -724,7 +725,9 @@
       <c r="D12" s="9">
         <v>1</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
@@ -737,7 +740,9 @@
       <c r="D13" s="9">
         <v>1</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="13">

</xml_diff>

<commit_message>
Added task to create JUnit Tests
</commit_message>
<xml_diff>
--- a/assignment8/src/Backlog/Sprint 1 Backlog.xlsx
+++ b/assignment8/src/Backlog/Sprint 1 Backlog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Very High</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>build class PaceCalculator.java</t>
+  </si>
+  <si>
+    <t>Create Junit tests for equivalent classes</t>
   </si>
 </sst>
 </file>
@@ -220,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -246,6 +249,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -554,7 +560,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,7 +757,7 @@
       <c r="C14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="14">
         <v>3</v>
       </c>
     </row>
@@ -762,6 +768,7 @@
       <c r="C15" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="13">
@@ -770,39 +777,49 @@
       <c r="C16" s="13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="14"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="13">
         <v>14</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="13">
         <v>15</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="14"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="13">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="13">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="13">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Burndown chart to backlog
</commit_message>
<xml_diff>
--- a/assignment8/src/Backlog/Sprint 1 Backlog.xlsx
+++ b/assignment8/src/Backlog/Sprint 1 Backlog.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14190" windowHeight="5505"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14190" windowHeight="5505" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="3" r:id="rId2"/>
+    <sheet name="Burndown Chart" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>Very High</t>
   </si>
@@ -92,10 +93,19 @@
     <t>build Class Time.java</t>
   </si>
   <si>
-    <t>build class PaceCalculator.java</t>
+    <t>Total</t>
   </si>
   <si>
-    <t>Create Junit tests for equivalent classes</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Do part 1 of assignment-8(research)</t>
+  </si>
+  <si>
+    <t>hrs</t>
+  </si>
+  <si>
+    <t>Remaining</t>
   </si>
 </sst>
 </file>
@@ -224,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -254,6 +264,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -269,6 +293,2033 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndown Chart'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Burndown Chart'!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>42669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42669</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42669</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42670</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42670</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42670</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42671</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42673</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42673</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42673</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42675</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42675</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42675</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burndown Chart'!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="400542408"/>
+        <c:axId val="400542800"/>
+      </c:barChart>
+      <c:dateAx>
+        <c:axId val="400542408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="400542800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="400542800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="400542408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Progress</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.42001459056495244"/>
+          <c:y val="1.8691588785046728E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndown Chart'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Burndown Chart'!$A$2:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>42669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42669</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42669</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42670</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42670</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42670</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42671</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42673</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42673</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42673</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42674</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42675</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>42675</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>42675</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burndown Chart'!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="400527904"/>
+        <c:axId val="387047592"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="400527904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="387047592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="387047592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Remaining</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Hours</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="400527904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="80" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8667750" cy="6298406"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3" title="Remaining Hrs"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -560,8 +2611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +2676,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>9</v>
@@ -640,13 +2691,13 @@
         <v>14</v>
       </c>
       <c r="D6" s="9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9">
         <v>4</v>
@@ -655,7 +2706,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>12</v>
@@ -685,7 +2736,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="9">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>10</v>
@@ -700,7 +2751,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>10</v>
@@ -811,24 +2862,14 @@
       <c r="B18" s="13">
         <v>15</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="14">
-        <v>2</v>
-      </c>
+      <c r="D18" s="14"/>
       <c r="E18" s="13"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="13">
         <v>16</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="14">
-        <v>4</v>
-      </c>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="13">
@@ -837,15 +2878,342 @@
       <c r="D20" s="14"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="13">
-        <v>18</v>
-      </c>
+      <c r="B21" s="13"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
+      <c r="C22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="13">
+        <f>SUM(D4:D21)</f>
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>42669</v>
+      </c>
+      <c r="B2" s="20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>42669</v>
+      </c>
+      <c r="B3" s="20">
+        <f>B2-C3</f>
+        <v>13.5</v>
+      </c>
+      <c r="C3" s="9">
+        <f>'Sprint 1'!D4</f>
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="18"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>42669</v>
+      </c>
+      <c r="B4" s="20">
+        <f>B3-C4</f>
+        <v>13</v>
+      </c>
+      <c r="C4" s="9">
+        <f>'Sprint 1'!D5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="18"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>42669</v>
+      </c>
+      <c r="B5" s="20">
+        <f>B4-C5</f>
+        <v>12.5</v>
+      </c>
+      <c r="C5" s="9">
+        <f>'Sprint 1'!D6</f>
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="9">
+        <v>3</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>42670</v>
+      </c>
+      <c r="B6" s="20">
+        <f>B5-C6</f>
+        <v>12</v>
+      </c>
+      <c r="C6" s="9">
+        <f>'Sprint 1'!D7</f>
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="9">
+        <v>4</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="18"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>42670</v>
+      </c>
+      <c r="B7" s="20">
+        <f>B6-C7</f>
+        <v>11.5</v>
+      </c>
+      <c r="C7" s="9">
+        <f>'Sprint 1'!D8</f>
+        <v>0.5</v>
+      </c>
+      <c r="D7" s="9">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="18"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>42670</v>
+      </c>
+      <c r="B8" s="20">
+        <f>B7-C8</f>
+        <v>11</v>
+      </c>
+      <c r="C8" s="9">
+        <f>'Sprint 1'!D9</f>
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="9">
+        <v>6</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="18"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>42671</v>
+      </c>
+      <c r="B9" s="20">
+        <f>B8-C9</f>
+        <v>9</v>
+      </c>
+      <c r="C9" s="9">
+        <f>'Sprint 1'!D10</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="9">
+        <v>7</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="18"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>42673</v>
+      </c>
+      <c r="B10" s="20">
+        <f>B9-C10</f>
+        <v>8</v>
+      </c>
+      <c r="C10" s="9">
+        <f>'Sprint 1'!D11</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
+        <v>8</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>42673</v>
+      </c>
+      <c r="B11" s="20">
+        <f>B10-C11</f>
+        <v>7</v>
+      </c>
+      <c r="C11" s="9">
+        <f>'Sprint 1'!D12</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="9">
+        <v>9</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>42673</v>
+      </c>
+      <c r="B12" s="20">
+        <f>B11-C12</f>
+        <v>6</v>
+      </c>
+      <c r="C12" s="9">
+        <f>'Sprint 1'!D13</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="9">
+        <v>10</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>42674</v>
+      </c>
+      <c r="B13" s="20">
+        <f>B12-C13</f>
+        <v>3</v>
+      </c>
+      <c r="C13" s="9">
+        <f>'Sprint 1'!D14</f>
+        <v>3</v>
+      </c>
+      <c r="D13" s="13">
+        <v>11</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>42675</v>
+      </c>
+      <c r="B14" s="20">
+        <f>B13-C14</f>
+        <v>2</v>
+      </c>
+      <c r="C14" s="9">
+        <f>'Sprint 1'!D15</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="13">
+        <v>12</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>42675</v>
+      </c>
+      <c r="B15" s="20">
+        <f>B14-C15</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="9">
+        <f>'Sprint 1'!D16</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="13">
+        <v>13</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>42675</v>
+      </c>
+      <c r="B16" s="20">
+        <f>B15-C16</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="9">
+        <f>'Sprint 1'!D17</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="13">
+        <v>14</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new taskings for GUI
</commit_message>
<xml_diff>
--- a/assignment8/src/Backlog/Sprint 1 Backlog.xlsx
+++ b/assignment8/src/Backlog/Sprint 1 Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14190" windowHeight="5505" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14190" windowHeight="5505"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>Very High</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Remaining</t>
+  </si>
+  <si>
+    <t>Updated GUI to refereence utility class</t>
+  </si>
+  <si>
+    <t>Updated GUI for correct calculations</t>
   </si>
 </sst>
 </file>
@@ -310,7 +316,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -490,11 +495,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="400542408"/>
-        <c:axId val="400542800"/>
+        <c:axId val="875177152"/>
+        <c:axId val="875188032"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="400542408"/>
+        <c:axId val="875177152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -537,14 +542,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400542800"/>
+        <c:crossAx val="875188032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="400542800"/>
+        <c:axId val="875188032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -595,7 +600,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400542408"/>
+        <c:crossAx val="875177152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -862,11 +867,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="400527904"/>
-        <c:axId val="387047592"/>
+        <c:axId val="875183136"/>
+        <c:axId val="875183680"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="400527904"/>
+        <c:axId val="875183136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,14 +984,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387047592"/>
+        <c:crossAx val="875183680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="387047592"/>
+        <c:axId val="875183680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1104,7 +1109,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400527904"/>
+        <c:crossAx val="875183136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2609,10 +2614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2855,30 +2860,47 @@
         <v>1</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="13">
         <v>15</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="13"/>
+      <c r="C18" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="14">
+        <v>2</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="13">
         <v>16</v>
       </c>
-      <c r="D19" s="14"/>
+      <c r="C19" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="14">
+        <v>2</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="13">
         <v>17</v>
       </c>
       <c r="D20" s="14"/>
+      <c r="E20" s="13"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="13"/>
+      <c r="E21" s="13"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="13"/>
@@ -2887,8 +2909,30 @@
       </c>
       <c r="D22" s="13">
         <f>SUM(D4:D21)</f>
-        <v>14</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="13"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="13"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2900,7 +2944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2936,7 +2980,7 @@
         <v>42669</v>
       </c>
       <c r="B3" s="20">
-        <f>B2-C3</f>
+        <f t="shared" ref="B3:B16" si="0">B2-C3</f>
         <v>13.5</v>
       </c>
       <c r="C3" s="9">
@@ -2956,7 +3000,7 @@
         <v>42669</v>
       </c>
       <c r="B4" s="20">
-        <f>B3-C4</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C4" s="9">
@@ -2976,7 +3020,7 @@
         <v>42669</v>
       </c>
       <c r="B5" s="20">
-        <f>B4-C5</f>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
       <c r="C5" s="9">
@@ -2996,7 +3040,7 @@
         <v>42670</v>
       </c>
       <c r="B6" s="20">
-        <f>B5-C6</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C6" s="9">
@@ -3016,7 +3060,7 @@
         <v>42670</v>
       </c>
       <c r="B7" s="20">
-        <f>B6-C7</f>
+        <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
       <c r="C7" s="9">
@@ -3036,7 +3080,7 @@
         <v>42670</v>
       </c>
       <c r="B8" s="20">
-        <f>B7-C8</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C8" s="9">
@@ -3056,7 +3100,7 @@
         <v>42671</v>
       </c>
       <c r="B9" s="20">
-        <f>B8-C9</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C9" s="9">
@@ -3076,7 +3120,7 @@
         <v>42673</v>
       </c>
       <c r="B10" s="20">
-        <f>B9-C10</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="C10" s="9">
@@ -3096,7 +3140,7 @@
         <v>42673</v>
       </c>
       <c r="B11" s="20">
-        <f>B10-C11</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C11" s="9">
@@ -3116,7 +3160,7 @@
         <v>42673</v>
       </c>
       <c r="B12" s="20">
-        <f>B11-C12</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C12" s="9">
@@ -3136,7 +3180,7 @@
         <v>42674</v>
       </c>
       <c r="B13" s="20">
-        <f>B12-C13</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C13" s="9">
@@ -3156,7 +3200,7 @@
         <v>42675</v>
       </c>
       <c r="B14" s="20">
-        <f>B13-C14</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C14" s="9">
@@ -3176,7 +3220,7 @@
         <v>42675</v>
       </c>
       <c r="B15" s="20">
-        <f>B14-C15</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C15" s="9">
@@ -3196,7 +3240,7 @@
         <v>42675</v>
       </c>
       <c r="B16" s="20">
-        <f>B15-C16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C16" s="9">

</xml_diff>